<commit_message>
fix: recopilacion de datos kine y fisioterapia rem BS
</commit_message>
<xml_diff>
--- a/RECIBIDO/EU/urgencias05.xlsx
+++ b/RECIBIDO/EU/urgencias05.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BoxEnfermera\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pie diabético\Desktop\Main\ESTADISTICAS\SERIES_A\2025\05\RECIBIDO\EU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBB43F5-B00B-4C6F-ACF7-9AA892F2B356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBD3EDB-536C-4A0A-8B07-BFAB9C037FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REMA" sheetId="1" r:id="rId1"/>
     <sheet name="REMB" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -402,7 +407,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +444,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="76">
     <border>
@@ -1361,7 +1372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1603,59 +1614,29 @@
     <xf numFmtId="165" fontId="13" fillId="4" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1663,6 +1644,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1674,16 +1685,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1691,6 +1702,15 @@
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="7" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1907,9 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
@@ -1959,23 +1980,23 @@
     <row r="1" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="141"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="141"/>
-      <c r="O3" s="142"/>
+      <c r="A3" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="121"/>
     </row>
     <row r="4" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2024,134 +2045,134 @@
       <c r="AN6" s="7"/>
     </row>
     <row r="7" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="145" t="s">
+      <c r="A7" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="124"/>
-      <c r="C7" s="123" t="s">
+      <c r="B7" s="123"/>
+      <c r="C7" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="128"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="121" t="s">
+      <c r="D7" s="129"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="130"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="130"/>
-      <c r="Q7" s="130"/>
-      <c r="R7" s="130"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="130"/>
-      <c r="U7" s="130"/>
-      <c r="V7" s="130"/>
-      <c r="W7" s="130"/>
-      <c r="X7" s="130"/>
-      <c r="Y7" s="130"/>
-      <c r="Z7" s="130"/>
-      <c r="AA7" s="130"/>
-      <c r="AB7" s="130"/>
-      <c r="AC7" s="130"/>
-      <c r="AD7" s="130"/>
-      <c r="AE7" s="130"/>
-      <c r="AF7" s="130"/>
-      <c r="AG7" s="130"/>
-      <c r="AH7" s="130"/>
-      <c r="AI7" s="130"/>
-      <c r="AJ7" s="130"/>
-      <c r="AK7" s="130"/>
-      <c r="AL7" s="130"/>
-      <c r="AM7" s="122"/>
-      <c r="AN7" s="146" t="s">
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="132"/>
+      <c r="T7" s="132"/>
+      <c r="U7" s="132"/>
+      <c r="V7" s="132"/>
+      <c r="W7" s="132"/>
+      <c r="X7" s="132"/>
+      <c r="Y7" s="132"/>
+      <c r="Z7" s="132"/>
+      <c r="AA7" s="132"/>
+      <c r="AB7" s="132"/>
+      <c r="AC7" s="132"/>
+      <c r="AD7" s="132"/>
+      <c r="AE7" s="132"/>
+      <c r="AF7" s="132"/>
+      <c r="AG7" s="132"/>
+      <c r="AH7" s="132"/>
+      <c r="AI7" s="132"/>
+      <c r="AJ7" s="132"/>
+      <c r="AK7" s="132"/>
+      <c r="AL7" s="132"/>
+      <c r="AM7" s="133"/>
+      <c r="AN7" s="134" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="125"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="121" t="s">
+      <c r="A8" s="124"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="122"/>
-      <c r="H8" s="121" t="s">
+      <c r="G8" s="133"/>
+      <c r="H8" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="122"/>
-      <c r="J8" s="121" t="s">
+      <c r="I8" s="133"/>
+      <c r="J8" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="122"/>
-      <c r="L8" s="121" t="s">
+      <c r="K8" s="133"/>
+      <c r="L8" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="122"/>
-      <c r="N8" s="121" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="122"/>
-      <c r="P8" s="131" t="s">
+      <c r="O8" s="133"/>
+      <c r="P8" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="122"/>
-      <c r="R8" s="131" t="s">
+      <c r="Q8" s="133"/>
+      <c r="R8" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="122"/>
-      <c r="T8" s="131" t="s">
+      <c r="S8" s="133"/>
+      <c r="T8" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="122"/>
-      <c r="V8" s="131" t="s">
+      <c r="U8" s="133"/>
+      <c r="V8" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="W8" s="122"/>
-      <c r="X8" s="131" t="s">
+      <c r="W8" s="133"/>
+      <c r="X8" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="Y8" s="122"/>
-      <c r="Z8" s="131" t="s">
+      <c r="Y8" s="133"/>
+      <c r="Z8" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="AA8" s="122"/>
-      <c r="AB8" s="131" t="s">
+      <c r="AA8" s="133"/>
+      <c r="AB8" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="122"/>
-      <c r="AD8" s="149" t="s">
+      <c r="AC8" s="133"/>
+      <c r="AD8" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="AE8" s="130"/>
-      <c r="AF8" s="131" t="s">
+      <c r="AE8" s="132"/>
+      <c r="AF8" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="AG8" s="122"/>
-      <c r="AH8" s="149" t="s">
+      <c r="AG8" s="133"/>
+      <c r="AH8" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="AI8" s="130"/>
-      <c r="AJ8" s="131" t="s">
+      <c r="AI8" s="132"/>
+      <c r="AJ8" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="AK8" s="122"/>
-      <c r="AL8" s="149" t="s">
+      <c r="AK8" s="133"/>
+      <c r="AL8" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="122"/>
-      <c r="AN8" s="147"/>
+      <c r="AM8" s="133"/>
+      <c r="AN8" s="135"/>
     </row>
     <row r="9" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="120"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
@@ -2263,13 +2284,13 @@
       <c r="AM9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AN9" s="148"/>
+      <c r="AN9" s="136"/>
     </row>
     <row r="10" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="132" t="s">
+      <c r="A10" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="133"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="16">
         <f>SUM(D10+E10)</f>
         <v>0</v>
@@ -2387,10 +2408,10 @@
       <c r="AN10" s="23"/>
     </row>
     <row r="11" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="142"/>
       <c r="C11" s="24">
         <v>0</v>
       </c>
@@ -2503,10 +2524,10 @@
       <c r="AN11" s="31"/>
     </row>
     <row r="12" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="138"/>
+      <c r="B12" s="145"/>
       <c r="C12" s="32">
         <f>SUM(D12+E12)</f>
         <v>0</v>
@@ -2635,12 +2656,12 @@
       <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="130"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="122"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="133"/>
       <c r="E15" s="43" t="s">
         <v>31</v>
       </c>
@@ -2652,11 +2673,11 @@
       <c r="A16" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="130"/>
-      <c r="D16" s="122"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="133"/>
       <c r="E16" s="44">
         <v>0</v>
       </c>
@@ -2667,23 +2688,23 @@
     <row r="17" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="140" t="s">
+      <c r="A19" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="141"/>
-      <c r="C19" s="141"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="141"/>
-      <c r="F19" s="141"/>
-      <c r="G19" s="141"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
-      <c r="L19" s="141"/>
-      <c r="M19" s="141"/>
-      <c r="N19" s="141"/>
-      <c r="O19" s="142"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="120"/>
+      <c r="O19" s="121"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="45"/>
       <c r="R19" s="45"/>
@@ -2714,85 +2735,85 @@
       <c r="O21" s="47"/>
     </row>
     <row r="22" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="143" t="s">
+      <c r="A22" s="148" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="141"/>
-      <c r="L22" s="141"/>
-      <c r="M22" s="141"/>
-      <c r="N22" s="141"/>
-      <c r="O22" s="142"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="120"/>
+      <c r="N22" s="120"/>
+      <c r="O22" s="121"/>
       <c r="P22" s="48"/>
       <c r="Q22" s="48"/>
     </row>
     <row r="23" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="123" t="s">
+      <c r="B23" s="123"/>
+      <c r="C23" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="128"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="121" t="s">
+      <c r="D23" s="129"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="130"/>
-      <c r="H23" s="130"/>
-      <c r="I23" s="130"/>
-      <c r="J23" s="130"/>
-      <c r="K23" s="130"/>
-      <c r="L23" s="130"/>
-      <c r="M23" s="130"/>
-      <c r="N23" s="130"/>
-      <c r="O23" s="130"/>
-      <c r="P23" s="130"/>
-      <c r="Q23" s="122"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="132"/>
+      <c r="K23" s="132"/>
+      <c r="L23" s="132"/>
+      <c r="M23" s="132"/>
+      <c r="N23" s="132"/>
+      <c r="O23" s="132"/>
+      <c r="P23" s="132"/>
+      <c r="Q23" s="133"/>
     </row>
     <row r="24" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="125"/>
-      <c r="B24" s="126"/>
-      <c r="C24" s="127"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="121" t="s">
+      <c r="A24" s="124"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="122"/>
-      <c r="H24" s="121" t="s">
+      <c r="G24" s="133"/>
+      <c r="H24" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="122"/>
-      <c r="J24" s="121" t="s">
+      <c r="I24" s="133"/>
+      <c r="J24" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="122"/>
-      <c r="L24" s="121" t="s">
+      <c r="K24" s="133"/>
+      <c r="L24" s="131" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="122"/>
-      <c r="N24" s="121" t="s">
+      <c r="M24" s="133"/>
+      <c r="N24" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="O24" s="122"/>
-      <c r="P24" s="121" t="s">
+      <c r="O24" s="133"/>
+      <c r="P24" s="131" t="s">
         <v>45</v>
       </c>
-      <c r="Q24" s="122"/>
+      <c r="Q24" s="133"/>
     </row>
     <row r="25" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="127"/>
-      <c r="B25" s="120"/>
+      <c r="A25" s="126"/>
+      <c r="B25" s="127"/>
       <c r="C25" s="49" t="s">
         <v>23</v>
       </c>
@@ -2840,10 +2861,10 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="132" t="s">
+      <c r="A26" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="133"/>
+      <c r="B26" s="140"/>
       <c r="C26" s="54">
         <v>0</v>
       </c>
@@ -2891,10 +2912,10 @@
       </c>
     </row>
     <row r="27" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="134" t="s">
+      <c r="A27" s="141" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="135"/>
+      <c r="B27" s="142"/>
       <c r="C27" s="61">
         <v>20</v>
       </c>
@@ -2942,10 +2963,10 @@
       </c>
     </row>
     <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="120"/>
+      <c r="B28" s="127"/>
       <c r="C28" s="67">
         <v>0</v>
       </c>
@@ -2993,10 +3014,10 @@
       </c>
     </row>
     <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="122"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="73">
         <v>20</v>
       </c>
@@ -4036,6 +4057,32 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A23:B25"/>
+    <mergeCell ref="C23:E24"/>
+    <mergeCell ref="F23:Q23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="A22:O22"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A7:B9"/>
     <mergeCell ref="C7:E8"/>
@@ -4052,32 +4099,6 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:U8"/>
     <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="A22:O22"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A23:B25"/>
-    <mergeCell ref="C23:E24"/>
-    <mergeCell ref="F23:Q23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="A3 A6:AN6 A7 C7 AN7 F7:F8 H8 J8 L8 N8 P8 R8 T8 V8 X8 Z8 AB8 AD8 AF8 AH8 AJ8 AL8 C9:AM9 A10:A12 C10:AN12 A14:F14 A15 A16:B16 E15:F16 A19 P19:Y19 P22:Q22 A22:A23 C23 F23:F24 H24 J24 L24 N24 A26:A29 A30:Q30 C25:O29 Q25:Q29 P24:P29" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4092,18 +4113,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="243.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
@@ -4172,13 +4193,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="85">
+      <c r="A7" s="162">
         <v>1602225</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="163" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="87">
+      <c r="C7" s="164">
         <v>11</v>
       </c>
     </row>
@@ -5423,6 +5444,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5484,134 +5506,134 @@
       <c r="AN2" s="7"/>
     </row>
     <row r="3" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="123" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="128"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="121" t="s">
+      <c r="D3" s="129"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-      <c r="O3" s="130"/>
-      <c r="P3" s="130"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="130"/>
-      <c r="T3" s="130"/>
-      <c r="U3" s="130"/>
-      <c r="V3" s="130"/>
-      <c r="W3" s="130"/>
-      <c r="X3" s="130"/>
-      <c r="Y3" s="130"/>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="130"/>
-      <c r="AB3" s="130"/>
-      <c r="AC3" s="130"/>
-      <c r="AD3" s="130"/>
-      <c r="AE3" s="130"/>
-      <c r="AF3" s="130"/>
-      <c r="AG3" s="130"/>
-      <c r="AH3" s="130"/>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="130"/>
-      <c r="AK3" s="130"/>
-      <c r="AL3" s="130"/>
-      <c r="AM3" s="122"/>
-      <c r="AN3" s="146" t="s">
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="U3" s="132"/>
+      <c r="V3" s="132"/>
+      <c r="W3" s="132"/>
+      <c r="X3" s="132"/>
+      <c r="Y3" s="132"/>
+      <c r="Z3" s="132"/>
+      <c r="AA3" s="132"/>
+      <c r="AB3" s="132"/>
+      <c r="AC3" s="132"/>
+      <c r="AD3" s="132"/>
+      <c r="AE3" s="132"/>
+      <c r="AF3" s="132"/>
+      <c r="AG3" s="132"/>
+      <c r="AH3" s="132"/>
+      <c r="AI3" s="132"/>
+      <c r="AJ3" s="132"/>
+      <c r="AK3" s="132"/>
+      <c r="AL3" s="132"/>
+      <c r="AM3" s="133"/>
+      <c r="AN3" s="134" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="125"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="121" t="s">
+      <c r="A4" s="124"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="122"/>
-      <c r="H4" s="121" t="s">
+      <c r="G4" s="133"/>
+      <c r="H4" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="122"/>
-      <c r="J4" s="121" t="s">
+      <c r="I4" s="133"/>
+      <c r="J4" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="122"/>
-      <c r="L4" s="121" t="s">
+      <c r="K4" s="133"/>
+      <c r="L4" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="122"/>
-      <c r="N4" s="121" t="s">
+      <c r="M4" s="133"/>
+      <c r="N4" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="122"/>
-      <c r="P4" s="131" t="s">
+      <c r="O4" s="133"/>
+      <c r="P4" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="131" t="s">
+      <c r="Q4" s="133"/>
+      <c r="R4" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="122"/>
-      <c r="T4" s="131" t="s">
+      <c r="S4" s="133"/>
+      <c r="T4" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="U4" s="122"/>
-      <c r="V4" s="131" t="s">
+      <c r="U4" s="133"/>
+      <c r="V4" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="122"/>
-      <c r="X4" s="131" t="s">
+      <c r="W4" s="133"/>
+      <c r="X4" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="Y4" s="122"/>
-      <c r="Z4" s="131" t="s">
+      <c r="Y4" s="133"/>
+      <c r="Z4" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="AA4" s="122"/>
-      <c r="AB4" s="131" t="s">
+      <c r="AA4" s="133"/>
+      <c r="AB4" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="AC4" s="122"/>
-      <c r="AD4" s="149" t="s">
+      <c r="AC4" s="133"/>
+      <c r="AD4" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="AE4" s="130"/>
-      <c r="AF4" s="131" t="s">
+      <c r="AE4" s="132"/>
+      <c r="AF4" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="AG4" s="122"/>
-      <c r="AH4" s="149" t="s">
+      <c r="AG4" s="133"/>
+      <c r="AH4" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="131" t="s">
+      <c r="AI4" s="132"/>
+      <c r="AJ4" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="AK4" s="122"/>
-      <c r="AL4" s="149" t="s">
+      <c r="AK4" s="133"/>
+      <c r="AL4" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="AM4" s="122"/>
-      <c r="AN4" s="147"/>
+      <c r="AM4" s="133"/>
+      <c r="AN4" s="135"/>
     </row>
     <row r="5" spans="1:40" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="127"/>
-      <c r="B5" s="120"/>
+      <c r="A5" s="126"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="12" t="s">
         <v>23</v>
       </c>
@@ -5723,13 +5745,13 @@
       <c r="AM5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AN5" s="148"/>
+      <c r="AN5" s="136"/>
     </row>
     <row r="6" spans="1:40" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="158" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="133"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
@@ -5773,7 +5795,7 @@
       <c r="A7" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="135"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="24"/>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -5817,7 +5839,7 @@
       <c r="A8" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="138"/>
+      <c r="B8" s="145"/>
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34"/>
@@ -5869,12 +5891,12 @@
       <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="130"/>
-      <c r="C11" s="130"/>
-      <c r="D11" s="122"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="133"/>
       <c r="E11" s="102" t="s">
         <v>31</v>
       </c>
@@ -5889,8 +5911,8 @@
       <c r="B12" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="122"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="133"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
     </row>
@@ -5941,64 +5963,64 @@
       <c r="AN15" s="47"/>
     </row>
     <row r="16" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="123" t="s">
+      <c r="A16" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="124"/>
-      <c r="C16" s="123" t="s">
+      <c r="B16" s="123"/>
+      <c r="C16" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="128"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="121" t="s">
+      <c r="D16" s="129"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
-      <c r="K16" s="130"/>
-      <c r="L16" s="130"/>
-      <c r="M16" s="130"/>
-      <c r="N16" s="130"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="130"/>
-      <c r="Q16" s="122"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="132"/>
+      <c r="K16" s="132"/>
+      <c r="L16" s="132"/>
+      <c r="M16" s="132"/>
+      <c r="N16" s="132"/>
+      <c r="O16" s="132"/>
+      <c r="P16" s="132"/>
+      <c r="Q16" s="133"/>
     </row>
     <row r="17" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="125"/>
-      <c r="B17" s="126"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="121" t="s">
+      <c r="A17" s="124"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="122"/>
-      <c r="H17" s="121" t="s">
+      <c r="G17" s="133"/>
+      <c r="H17" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="122"/>
-      <c r="J17" s="121" t="s">
+      <c r="I17" s="133"/>
+      <c r="J17" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="122"/>
-      <c r="L17" s="121" t="s">
+      <c r="K17" s="133"/>
+      <c r="L17" s="131" t="s">
         <v>43</v>
       </c>
-      <c r="M17" s="122"/>
-      <c r="N17" s="121" t="s">
+      <c r="M17" s="133"/>
+      <c r="N17" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="O17" s="122"/>
-      <c r="P17" s="121" t="s">
+      <c r="O17" s="133"/>
+      <c r="P17" s="131" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="122"/>
+      <c r="Q17" s="133"/>
     </row>
     <row r="18" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
-      <c r="B18" s="120"/>
+      <c r="A18" s="126"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="105" t="s">
         <v>23</v>
       </c>
@@ -6046,10 +6068,10 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="133"/>
+      <c r="B19" s="140"/>
       <c r="C19" s="109"/>
       <c r="D19" s="110"/>
       <c r="E19" s="111"/>
@@ -6067,10 +6089,10 @@
       <c r="Q19" s="60"/>
     </row>
     <row r="20" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="157" t="s">
+      <c r="A20" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="135"/>
+      <c r="B20" s="142"/>
       <c r="C20" s="112"/>
       <c r="D20" s="113"/>
       <c r="E20" s="114"/>
@@ -6088,10 +6110,10 @@
       <c r="Q20" s="65"/>
     </row>
     <row r="21" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="120"/>
+      <c r="B21" s="127"/>
       <c r="C21" s="115"/>
       <c r="D21" s="116"/>
       <c r="E21" s="117"/>
@@ -6109,10 +6131,10 @@
       <c r="Q21" s="71"/>
     </row>
     <row r="22" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="122"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="73"/>
       <c r="D22" s="74"/>
       <c r="E22" s="75"/>
@@ -7109,24 +7131,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="F16:Q16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A16:B18"/>
-    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="F3:AM3"/>
     <mergeCell ref="AN3:AN5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
@@ -7143,11 +7152,24 @@
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="F3:AM3"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A16:B18"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="F16:Q16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="A15:Q15 A16 C16 F16:F17 H17 J17 L17 N17 P17 A19:A22 C18:Q22" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>